<commit_message>
Fixes made with Arnaldo
</commit_message>
<xml_diff>
--- a/ArnaldoDiBianco/Lista_materiale3.xlsx
+++ b/ArnaldoDiBianco/Lista_materiale3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sources\Local\ArnaldoDiBianco\ArnaldoDiBianco\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0132B128-062A-45E5-9B07-B293B9174C3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFBB8EEB-ABD3-4BB7-82D8-7211CF93283E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="16608" windowHeight="8856" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Utente" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
+    <comment ref="AG5" authorId="0" shapeId="0" xr:uid="{612D763F-EDF6-4CB0-8005-6A053A355A9E}">
       <text>
         <r>
           <rPr>
@@ -593,7 +593,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="[$€-410]&quot; &quot;#,##0.00;[Red]&quot;-&quot;[$€-410]&quot; &quot;#,##0.00"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -744,6 +744,27 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="8" tint="0.39994506668294322"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -794,7 +815,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -927,22 +948,32 @@
     <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1645,9 +1676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMH1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="E76" sqref="E76"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1918,34 +1947,34 @@
       <c r="M14" s="3"/>
     </row>
     <row r="15" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="59"/>
-      <c r="B15" s="59"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="59"/>
-      <c r="K15" s="59"/>
-      <c r="L15" s="59"/>
-      <c r="M15" s="59"/>
+      <c r="A15" s="64"/>
+      <c r="B15" s="64"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="64"/>
+      <c r="F15" s="64"/>
+      <c r="G15" s="64"/>
+      <c r="H15" s="64"/>
+      <c r="I15" s="64"/>
+      <c r="J15" s="64"/>
+      <c r="K15" s="64"/>
+      <c r="L15" s="64"/>
+      <c r="M15" s="64"/>
     </row>
     <row r="16" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="59"/>
-      <c r="B16" s="59"/>
-      <c r="C16" s="59"/>
-      <c r="D16" s="59"/>
-      <c r="E16" s="59"/>
-      <c r="F16" s="59"/>
-      <c r="G16" s="59"/>
-      <c r="H16" s="59"/>
-      <c r="I16" s="59"/>
-      <c r="J16" s="59"/>
-      <c r="K16" s="59"/>
-      <c r="L16" s="59"/>
-      <c r="M16" s="59"/>
+      <c r="A16" s="64"/>
+      <c r="B16" s="64"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="64"/>
+      <c r="F16" s="64"/>
+      <c r="G16" s="64"/>
+      <c r="H16" s="64"/>
+      <c r="I16" s="64"/>
+      <c r="J16" s="64"/>
+      <c r="K16" s="64"/>
+      <c r="L16" s="64"/>
+      <c r="M16" s="64"/>
     </row>
     <row r="17" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17"/>
@@ -2201,38 +2230,38 @@
       <c r="M30" s="3"/>
     </row>
     <row r="31" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="59"/>
-      <c r="B31" s="59"/>
-      <c r="C31" s="59"/>
-      <c r="D31" s="59"/>
-      <c r="E31" s="59"/>
-      <c r="F31" s="59"/>
-      <c r="G31" s="59"/>
-      <c r="H31" s="59"/>
-      <c r="I31" s="59"/>
-      <c r="J31" s="59"/>
-      <c r="K31" s="59"/>
-      <c r="L31" s="59"/>
-      <c r="M31" s="59"/>
+      <c r="A31" s="64"/>
+      <c r="B31" s="64"/>
+      <c r="C31" s="64"/>
+      <c r="D31" s="64"/>
+      <c r="E31" s="64"/>
+      <c r="F31" s="64"/>
+      <c r="G31" s="64"/>
+      <c r="H31" s="64"/>
+      <c r="I31" s="64"/>
+      <c r="J31" s="64"/>
+      <c r="K31" s="64"/>
+      <c r="L31" s="64"/>
+      <c r="M31" s="64"/>
     </row>
     <row r="32" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="59"/>
-      <c r="B32" s="59"/>
-      <c r="C32" s="59"/>
-      <c r="D32" s="59"/>
-      <c r="E32" s="59"/>
-      <c r="F32" s="59"/>
-      <c r="G32" s="59"/>
-      <c r="H32" s="59"/>
-      <c r="I32" s="59"/>
-      <c r="J32" s="59"/>
-      <c r="K32" s="59"/>
-      <c r="L32" s="59"/>
-      <c r="M32" s="59"/>
+      <c r="A32" s="64"/>
+      <c r="B32" s="64"/>
+      <c r="C32" s="64"/>
+      <c r="D32" s="64"/>
+      <c r="E32" s="64"/>
+      <c r="F32" s="64"/>
+      <c r="G32" s="64"/>
+      <c r="H32" s="64"/>
+      <c r="I32" s="64"/>
+      <c r="J32" s="64"/>
+      <c r="K32" s="64"/>
+      <c r="L32" s="64"/>
+      <c r="M32" s="64"/>
     </row>
     <row r="33" spans="1:16" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="58"/>
-      <c r="B33" s="58"/>
+      <c r="A33" s="66"/>
+      <c r="B33" s="66"/>
       <c r="C33" s="2" t="s">
         <v>0</v>
       </c>
@@ -2242,8 +2271,8 @@
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="14"/>
-      <c r="H33" s="59"/>
-      <c r="I33" s="59"/>
+      <c r="H33" s="64"/>
+      <c r="I33" s="64"/>
       <c r="J33" s="2" t="s">
         <v>0</v>
       </c>
@@ -2254,8 +2283,8 @@
       <c r="M33" s="3"/>
     </row>
     <row r="34" spans="1:16" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="58"/>
-      <c r="B34" s="58"/>
+      <c r="A34" s="66"/>
+      <c r="B34" s="66"/>
       <c r="C34" s="2" t="s">
         <v>1</v>
       </c>
@@ -2265,8 +2294,8 @@
       </c>
       <c r="F34" s="3"/>
       <c r="G34" s="14"/>
-      <c r="H34" s="59"/>
-      <c r="I34" s="59"/>
+      <c r="H34" s="64"/>
+      <c r="I34" s="64"/>
       <c r="J34" s="2" t="s">
         <v>1</v>
       </c>
@@ -2277,23 +2306,23 @@
       <c r="M34" s="3"/>
     </row>
     <row r="35" spans="1:16" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="58"/>
-      <c r="B35" s="58"/>
+      <c r="A35" s="66"/>
+      <c r="B35" s="66"/>
       <c r="C35" s="2"/>
       <c r="D35" s="3"/>
       <c r="E35" s="2"/>
       <c r="F35" s="3"/>
       <c r="G35" s="14"/>
-      <c r="H35" s="59"/>
-      <c r="I35" s="59"/>
+      <c r="H35" s="64"/>
+      <c r="I35" s="64"/>
       <c r="J35" s="2"/>
       <c r="K35" s="3"/>
       <c r="L35" s="2"/>
       <c r="M35" s="3"/>
     </row>
     <row r="36" spans="1:16" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="58"/>
-      <c r="B36" s="58"/>
+      <c r="A36" s="66"/>
+      <c r="B36" s="66"/>
       <c r="C36" s="2" t="s">
         <v>0</v>
       </c>
@@ -2303,8 +2332,8 @@
       </c>
       <c r="F36" s="3"/>
       <c r="G36" s="14"/>
-      <c r="H36" s="59"/>
-      <c r="I36" s="59"/>
+      <c r="H36" s="64"/>
+      <c r="I36" s="64"/>
       <c r="J36" s="2" t="s">
         <v>0</v>
       </c>
@@ -2317,8 +2346,8 @@
       <c r="P36" s="13"/>
     </row>
     <row r="37" spans="1:16" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="58"/>
-      <c r="B37" s="58"/>
+      <c r="A37" s="66"/>
+      <c r="B37" s="66"/>
       <c r="C37" s="2" t="s">
         <v>1</v>
       </c>
@@ -2328,8 +2357,8 @@
       </c>
       <c r="F37" s="3"/>
       <c r="G37" s="14"/>
-      <c r="H37" s="59"/>
-      <c r="I37" s="59"/>
+      <c r="H37" s="64"/>
+      <c r="I37" s="64"/>
       <c r="J37" s="2" t="s">
         <v>1</v>
       </c>
@@ -2342,15 +2371,15 @@
       <c r="P37" s="13"/>
     </row>
     <row r="38" spans="1:16" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="58"/>
-      <c r="B38" s="58"/>
+      <c r="A38" s="66"/>
+      <c r="B38" s="66"/>
       <c r="C38" s="9"/>
       <c r="D38" s="3"/>
       <c r="E38" s="9"/>
       <c r="F38" s="3"/>
       <c r="G38" s="13"/>
-      <c r="H38" s="59"/>
-      <c r="I38" s="59"/>
+      <c r="H38" s="64"/>
+      <c r="I38" s="64"/>
       <c r="J38" s="9"/>
       <c r="K38" s="3"/>
       <c r="L38" s="9"/>
@@ -2359,8 +2388,8 @@
       <c r="P38" s="13"/>
     </row>
     <row r="39" spans="1:16" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="58"/>
-      <c r="B39" s="58"/>
+      <c r="A39" s="66"/>
+      <c r="B39" s="66"/>
       <c r="C39" s="2" t="s">
         <v>0</v>
       </c>
@@ -2370,8 +2399,8 @@
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="13"/>
-      <c r="H39" s="59"/>
-      <c r="I39" s="59"/>
+      <c r="H39" s="64"/>
+      <c r="I39" s="64"/>
       <c r="J39" s="2" t="s">
         <v>0</v>
       </c>
@@ -2384,8 +2413,8 @@
       <c r="P39" s="13"/>
     </row>
     <row r="40" spans="1:16" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="58"/>
-      <c r="B40" s="58"/>
+      <c r="A40" s="66"/>
+      <c r="B40" s="66"/>
       <c r="C40" s="2" t="s">
         <v>1</v>
       </c>
@@ -2395,8 +2424,8 @@
       </c>
       <c r="F40" s="3"/>
       <c r="G40" s="13"/>
-      <c r="H40" s="59"/>
-      <c r="I40" s="59"/>
+      <c r="H40" s="64"/>
+      <c r="I40" s="64"/>
       <c r="J40" s="2" t="s">
         <v>1</v>
       </c>
@@ -2408,23 +2437,23 @@
       <c r="P40" s="13"/>
     </row>
     <row r="41" spans="1:16" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="58"/>
-      <c r="B41" s="58"/>
+      <c r="A41" s="66"/>
+      <c r="B41" s="66"/>
       <c r="C41" s="2"/>
       <c r="D41" s="3"/>
       <c r="E41" s="2"/>
       <c r="F41" s="3"/>
       <c r="G41" s="13"/>
-      <c r="H41" s="59"/>
-      <c r="I41" s="59"/>
+      <c r="H41" s="64"/>
+      <c r="I41" s="64"/>
       <c r="J41" s="2"/>
       <c r="K41" s="3"/>
       <c r="L41" s="2"/>
       <c r="M41" s="3"/>
     </row>
     <row r="42" spans="1:16" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="58"/>
-      <c r="B42" s="58"/>
+      <c r="A42" s="66"/>
+      <c r="B42" s="66"/>
       <c r="C42" s="2" t="s">
         <v>0</v>
       </c>
@@ -2434,8 +2463,8 @@
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="13"/>
-      <c r="H42" s="59"/>
-      <c r="I42" s="59"/>
+      <c r="H42" s="64"/>
+      <c r="I42" s="64"/>
       <c r="J42" s="2" t="s">
         <v>0</v>
       </c>
@@ -2446,8 +2475,8 @@
       <c r="M42" s="3"/>
     </row>
     <row r="43" spans="1:16" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="58"/>
-      <c r="B43" s="58"/>
+      <c r="A43" s="66"/>
+      <c r="B43" s="66"/>
       <c r="C43" s="2" t="s">
         <v>1</v>
       </c>
@@ -2457,8 +2486,8 @@
       </c>
       <c r="F43" s="3"/>
       <c r="G43" s="13"/>
-      <c r="H43" s="59"/>
-      <c r="I43" s="59"/>
+      <c r="H43" s="64"/>
+      <c r="I43" s="64"/>
       <c r="J43" s="2" t="s">
         <v>1</v>
       </c>
@@ -2469,23 +2498,23 @@
       <c r="M43" s="3"/>
     </row>
     <row r="44" spans="1:16" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="58"/>
-      <c r="B44" s="58"/>
+      <c r="A44" s="66"/>
+      <c r="B44" s="66"/>
       <c r="C44" s="9"/>
       <c r="D44" s="3"/>
       <c r="E44" s="9"/>
       <c r="F44" s="3"/>
       <c r="G44" s="13"/>
-      <c r="H44" s="59"/>
-      <c r="I44" s="59"/>
+      <c r="H44" s="64"/>
+      <c r="I44" s="64"/>
       <c r="J44" s="9"/>
       <c r="K44" s="3"/>
       <c r="L44" s="9"/>
       <c r="M44" s="3"/>
     </row>
     <row r="45" spans="1:16" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="58"/>
-      <c r="B45" s="58"/>
+      <c r="A45" s="66"/>
+      <c r="B45" s="66"/>
       <c r="C45" s="2" t="s">
         <v>0</v>
       </c>
@@ -2495,8 +2524,8 @@
       </c>
       <c r="F45" s="3"/>
       <c r="G45" s="13"/>
-      <c r="H45" s="59"/>
-      <c r="I45" s="59"/>
+      <c r="H45" s="64"/>
+      <c r="I45" s="64"/>
       <c r="J45" s="2" t="s">
         <v>0</v>
       </c>
@@ -2507,8 +2536,8 @@
       <c r="M45" s="3"/>
     </row>
     <row r="46" spans="1:16" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="58"/>
-      <c r="B46" s="58"/>
+      <c r="A46" s="66"/>
+      <c r="B46" s="66"/>
       <c r="C46" s="2" t="s">
         <v>1</v>
       </c>
@@ -2518,8 +2547,8 @@
       </c>
       <c r="F46" s="3"/>
       <c r="G46" s="13"/>
-      <c r="H46" s="59"/>
-      <c r="I46" s="59"/>
+      <c r="H46" s="64"/>
+      <c r="I46" s="64"/>
       <c r="J46" s="2" t="s">
         <v>1</v>
       </c>
@@ -2530,38 +2559,38 @@
       <c r="M46" s="3"/>
     </row>
     <row r="47" spans="1:16" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="59"/>
-      <c r="B47" s="59"/>
-      <c r="C47" s="59"/>
-      <c r="D47" s="59"/>
-      <c r="E47" s="59"/>
-      <c r="F47" s="59"/>
-      <c r="G47" s="59"/>
-      <c r="H47" s="59"/>
-      <c r="I47" s="59"/>
-      <c r="J47" s="59"/>
-      <c r="K47" s="59"/>
-      <c r="L47" s="59"/>
-      <c r="M47" s="59"/>
+      <c r="A47" s="64"/>
+      <c r="B47" s="64"/>
+      <c r="C47" s="64"/>
+      <c r="D47" s="64"/>
+      <c r="E47" s="64"/>
+      <c r="F47" s="64"/>
+      <c r="G47" s="64"/>
+      <c r="H47" s="64"/>
+      <c r="I47" s="64"/>
+      <c r="J47" s="64"/>
+      <c r="K47" s="64"/>
+      <c r="L47" s="64"/>
+      <c r="M47" s="64"/>
     </row>
     <row r="48" spans="1:16" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="59"/>
-      <c r="B48" s="59"/>
-      <c r="C48" s="59"/>
-      <c r="D48" s="59"/>
-      <c r="E48" s="59"/>
-      <c r="F48" s="59"/>
-      <c r="G48" s="59"/>
-      <c r="H48" s="59"/>
-      <c r="I48" s="59"/>
-      <c r="J48" s="59"/>
-      <c r="K48" s="59"/>
-      <c r="L48" s="59"/>
-      <c r="M48" s="59"/>
+      <c r="A48" s="64"/>
+      <c r="B48" s="64"/>
+      <c r="C48" s="64"/>
+      <c r="D48" s="64"/>
+      <c r="E48" s="64"/>
+      <c r="F48" s="64"/>
+      <c r="G48" s="64"/>
+      <c r="H48" s="64"/>
+      <c r="I48" s="64"/>
+      <c r="J48" s="64"/>
+      <c r="K48" s="64"/>
+      <c r="L48" s="64"/>
+      <c r="M48" s="64"/>
     </row>
     <row r="49" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="58"/>
-      <c r="B49" s="58"/>
+      <c r="A49" s="66"/>
+      <c r="B49" s="66"/>
       <c r="C49" s="2" t="s">
         <v>0</v>
       </c>
@@ -2583,8 +2612,8 @@
       <c r="M49" s="3"/>
     </row>
     <row r="50" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="58"/>
-      <c r="B50" s="58"/>
+      <c r="A50" s="66"/>
+      <c r="B50" s="66"/>
       <c r="C50" s="2" t="s">
         <v>1</v>
       </c>
@@ -2606,8 +2635,8 @@
       <c r="M50" s="3"/>
     </row>
     <row r="51" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="58"/>
-      <c r="B51" s="58"/>
+      <c r="A51" s="66"/>
+      <c r="B51" s="66"/>
       <c r="C51" s="2"/>
       <c r="D51" s="3"/>
       <c r="E51" s="2"/>
@@ -2621,8 +2650,8 @@
       <c r="M51" s="3"/>
     </row>
     <row r="52" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="58"/>
-      <c r="B52" s="58"/>
+      <c r="A52" s="66"/>
+      <c r="B52" s="66"/>
       <c r="C52" s="2" t="s">
         <v>0</v>
       </c>
@@ -2644,8 +2673,8 @@
       <c r="M52" s="3"/>
     </row>
     <row r="53" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="58"/>
-      <c r="B53" s="58"/>
+      <c r="A53" s="66"/>
+      <c r="B53" s="66"/>
       <c r="C53" s="2" t="s">
         <v>1</v>
       </c>
@@ -2667,8 +2696,8 @@
       <c r="M53" s="3"/>
     </row>
     <row r="54" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="58"/>
-      <c r="B54" s="58"/>
+      <c r="A54" s="66"/>
+      <c r="B54" s="66"/>
       <c r="C54" s="9"/>
       <c r="D54" s="3"/>
       <c r="E54" s="9"/>
@@ -2680,8 +2709,8 @@
       <c r="M54" s="3"/>
     </row>
     <row r="55" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="58"/>
-      <c r="B55" s="58"/>
+      <c r="A55" s="66"/>
+      <c r="B55" s="66"/>
       <c r="C55" s="2" t="s">
         <v>0</v>
       </c>
@@ -2701,8 +2730,8 @@
       <c r="M55" s="3"/>
     </row>
     <row r="56" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="58"/>
-      <c r="B56" s="58"/>
+      <c r="A56" s="66"/>
+      <c r="B56" s="66"/>
       <c r="C56" s="2" t="s">
         <v>1</v>
       </c>
@@ -2722,8 +2751,8 @@
       <c r="M56" s="3"/>
     </row>
     <row r="57" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="58"/>
-      <c r="B57" s="58"/>
+      <c r="A57" s="66"/>
+      <c r="B57" s="66"/>
       <c r="C57" s="2"/>
       <c r="D57" s="3"/>
       <c r="E57" s="2"/>
@@ -2735,8 +2764,8 @@
       <c r="M57" s="3"/>
     </row>
     <row r="58" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="58"/>
-      <c r="B58" s="58"/>
+      <c r="A58" s="66"/>
+      <c r="B58" s="66"/>
       <c r="C58" s="2" t="s">
         <v>0</v>
       </c>
@@ -2756,8 +2785,8 @@
       <c r="M58" s="3"/>
     </row>
     <row r="59" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="58"/>
-      <c r="B59" s="58"/>
+      <c r="A59" s="66"/>
+      <c r="B59" s="66"/>
       <c r="C59" s="2" t="s">
         <v>1</v>
       </c>
@@ -2777,8 +2806,8 @@
       <c r="M59" s="3"/>
     </row>
     <row r="60" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="58"/>
-      <c r="B60" s="58"/>
+      <c r="A60" s="66"/>
+      <c r="B60" s="66"/>
       <c r="C60" s="9"/>
       <c r="D60" s="3"/>
       <c r="E60" s="9"/>
@@ -2790,8 +2819,8 @@
       <c r="M60" s="3"/>
     </row>
     <row r="61" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="58"/>
-      <c r="B61" s="58"/>
+      <c r="A61" s="66"/>
+      <c r="B61" s="66"/>
       <c r="C61" s="2" t="s">
         <v>0</v>
       </c>
@@ -2811,8 +2840,8 @@
       <c r="M61" s="3"/>
     </row>
     <row r="62" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="58"/>
-      <c r="B62" s="58"/>
+      <c r="A62" s="66"/>
+      <c r="B62" s="66"/>
       <c r="C62" s="2" t="s">
         <v>1</v>
       </c>
@@ -2831,57 +2860,57 @@
       <c r="M62" s="3"/>
     </row>
     <row r="63" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="59"/>
-      <c r="B63" s="59"/>
-      <c r="C63" s="59"/>
-      <c r="D63" s="59"/>
-      <c r="E63" s="59"/>
-      <c r="F63" s="59"/>
-      <c r="G63" s="59"/>
-      <c r="H63" s="59"/>
-      <c r="I63" s="59"/>
-      <c r="J63" s="59"/>
-      <c r="K63" s="59"/>
-      <c r="L63" s="59"/>
-      <c r="M63" s="59"/>
+      <c r="A63" s="64"/>
+      <c r="B63" s="64"/>
+      <c r="C63" s="64"/>
+      <c r="D63" s="64"/>
+      <c r="E63" s="64"/>
+      <c r="F63" s="64"/>
+      <c r="G63" s="64"/>
+      <c r="H63" s="64"/>
+      <c r="I63" s="64"/>
+      <c r="J63" s="64"/>
+      <c r="K63" s="64"/>
+      <c r="L63" s="64"/>
+      <c r="M63" s="64"/>
     </row>
     <row r="64" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="59"/>
-      <c r="B64" s="59"/>
-      <c r="C64" s="59"/>
-      <c r="D64" s="59"/>
-      <c r="E64" s="59"/>
-      <c r="F64" s="59"/>
-      <c r="G64" s="59"/>
-      <c r="H64" s="59"/>
-      <c r="I64" s="59"/>
-      <c r="J64" s="59"/>
-      <c r="K64" s="59"/>
-      <c r="L64" s="59"/>
-      <c r="M64" s="59"/>
+      <c r="A64" s="64"/>
+      <c r="B64" s="64"/>
+      <c r="C64" s="64"/>
+      <c r="D64" s="64"/>
+      <c r="E64" s="64"/>
+      <c r="F64" s="64"/>
+      <c r="G64" s="64"/>
+      <c r="H64" s="64"/>
+      <c r="I64" s="64"/>
+      <c r="J64" s="64"/>
+      <c r="K64" s="64"/>
+      <c r="L64" s="64"/>
+      <c r="M64" s="64"/>
     </row>
     <row r="65" spans="1:1022" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="59"/>
-      <c r="B65" s="59"/>
-      <c r="C65" s="59"/>
-      <c r="D65" s="59"/>
-      <c r="E65" s="59"/>
-      <c r="F65" s="59"/>
-      <c r="G65" s="59"/>
-      <c r="H65" s="59"/>
-      <c r="I65" s="59"/>
-      <c r="J65" s="59"/>
-      <c r="K65" s="59"/>
-      <c r="L65" s="59"/>
-      <c r="M65" s="59"/>
+      <c r="A65" s="64"/>
+      <c r="B65" s="64"/>
+      <c r="C65" s="64"/>
+      <c r="D65" s="64"/>
+      <c r="E65" s="64"/>
+      <c r="F65" s="64"/>
+      <c r="G65" s="64"/>
+      <c r="H65" s="64"/>
+      <c r="I65" s="64"/>
+      <c r="J65" s="64"/>
+      <c r="K65" s="64"/>
+      <c r="L65" s="64"/>
+      <c r="M65" s="64"/>
     </row>
     <row r="66" spans="1:1022" s="47" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="44"/>
       <c r="B66" s="44"/>
-      <c r="C66" s="60" t="s">
+      <c r="C66" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D66" s="60"/>
+      <c r="D66" s="63"/>
       <c r="E66" s="49">
         <f>Persiane!BC94</f>
         <v>0.58461538461538465</v>
@@ -3904,19 +3933,19 @@
     <row r="67" spans="1:1022" s="47" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="44"/>
       <c r="B67" s="44"/>
-      <c r="C67" s="61" t="s">
+      <c r="C67" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="D67" s="61"/>
+      <c r="D67" s="60"/>
       <c r="E67" s="49">
         <f>Finestre!BA62</f>
         <v>0</v>
       </c>
       <c r="I67" s="44"/>
-      <c r="N67" s="62" t="s">
+      <c r="N67" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="O67" s="62"/>
+      <c r="O67" s="65"/>
       <c r="P67" s="45">
         <f>Persiane!BC95</f>
         <v>1.1015384615384616</v>
@@ -4931,19 +4960,19 @@
     <row r="68" spans="1:1022" s="47" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="44"/>
       <c r="B68" s="44"/>
-      <c r="C68" s="61" t="s">
+      <c r="C68" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="D68" s="61"/>
+      <c r="D68" s="60"/>
       <c r="E68" s="49">
         <f>Finestre!BA64</f>
         <v>0</v>
       </c>
       <c r="I68" s="44"/>
-      <c r="N68" s="63" t="s">
+      <c r="N68" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="O68" s="63"/>
+      <c r="O68" s="59"/>
       <c r="P68" s="45">
         <f>Finestre!BA63</f>
         <v>0</v>
@@ -5958,19 +5987,19 @@
     <row r="69" spans="1:1022" s="47" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="44"/>
       <c r="B69" s="44"/>
-      <c r="C69" s="64" t="s">
+      <c r="C69" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="D69" s="64"/>
+      <c r="D69" s="58"/>
       <c r="E69" s="50">
         <f>P67+P68</f>
         <v>1.1015384615384616</v>
       </c>
       <c r="I69" s="44"/>
-      <c r="N69" s="65" t="s">
+      <c r="N69" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="O69" s="65"/>
+      <c r="O69" s="62"/>
       <c r="P69" s="45">
         <f>Persiane!BC100</f>
         <v>0</v>
@@ -6985,19 +7014,19 @@
     <row r="70" spans="1:1022" s="47" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="44"/>
       <c r="B70" s="44"/>
-      <c r="C70" s="64" t="s">
+      <c r="C70" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="D70" s="64"/>
+      <c r="D70" s="58"/>
       <c r="E70" s="50">
         <f>P71+P72</f>
         <v>0.18153846153846154</v>
       </c>
       <c r="I70" s="44"/>
-      <c r="N70" s="63" t="s">
+      <c r="N70" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="O70" s="63"/>
+      <c r="O70" s="59"/>
       <c r="P70" s="45">
         <f>Finestre!BA65</f>
         <v>0</v>
@@ -8012,19 +8041,19 @@
     <row r="71" spans="1:1022" s="47" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="44"/>
       <c r="B71" s="44"/>
-      <c r="C71" s="60" t="s">
+      <c r="C71" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="D71" s="60"/>
+      <c r="D71" s="63"/>
       <c r="E71" s="49">
         <f>Persiane!BC96</f>
         <v>0.1676923076923077</v>
       </c>
       <c r="I71" s="44"/>
-      <c r="N71" s="65" t="s">
+      <c r="N71" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="O71" s="65"/>
+      <c r="O71" s="62"/>
       <c r="P71" s="45">
         <f>Persiane!BC101</f>
         <v>0.18153846153846154</v>
@@ -9039,20 +9068,20 @@
     <row r="72" spans="1:1022" s="47" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="44"/>
       <c r="B72" s="44"/>
-      <c r="C72" s="64" t="s">
+      <c r="C72" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="D72" s="64"/>
+      <c r="D72" s="58"/>
       <c r="E72" s="50">
         <f>P69+P70</f>
         <v>0</v>
       </c>
       <c r="I72" s="44"/>
       <c r="J72" s="44"/>
-      <c r="N72" s="63" t="s">
+      <c r="N72" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="O72" s="63"/>
+      <c r="O72" s="59"/>
       <c r="P72" s="45">
         <f>Finestre!BA67</f>
         <v>0</v>
@@ -10067,10 +10096,10 @@
     <row r="73" spans="1:1022" s="47" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="44"/>
       <c r="B73" s="44"/>
-      <c r="C73" s="61" t="s">
+      <c r="C73" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="D73" s="61"/>
+      <c r="D73" s="60"/>
       <c r="E73" s="49">
         <f>Finestre!BA66</f>
         <v>0</v>
@@ -11093,10 +11122,10 @@
     <row r="74" spans="1:1022" s="47" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="44"/>
       <c r="B74" s="44"/>
-      <c r="C74" s="66" t="s">
+      <c r="C74" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="D74" s="66"/>
+      <c r="D74" s="61"/>
       <c r="E74" s="49">
         <f>Persiane!BC97</f>
         <v>0.25230769230769229</v>
@@ -12119,10 +12148,10 @@
     <row r="75" spans="1:1022" s="47" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="44"/>
       <c r="B75" s="44"/>
-      <c r="C75" s="66" t="s">
+      <c r="C75" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="D75" s="66"/>
+      <c r="D75" s="61"/>
       <c r="E75" s="49">
         <f>Persiane!BC98</f>
         <v>0.24</v>
@@ -13145,13 +13174,13 @@
     <row r="76" spans="1:1022" s="47" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="44"/>
       <c r="B76" s="44"/>
-      <c r="C76" s="66" t="s">
+      <c r="C76" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="D76" s="66"/>
+      <c r="D76" s="61"/>
       <c r="E76" s="49">
         <f>Persiane!BC99</f>
-        <v>-0.36923076923076925</v>
+        <v>2.2153846153846155</v>
       </c>
       <c r="I76" s="44"/>
       <c r="J76" s="44"/>
@@ -14171,10 +14200,10 @@
     <row r="77" spans="1:1022" s="47" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="44"/>
       <c r="B77" s="44"/>
-      <c r="C77" s="64" t="s">
+      <c r="C77" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="D77" s="64"/>
+      <c r="D77" s="58"/>
       <c r="E77" s="51"/>
       <c r="F77" s="48"/>
       <c r="G77" s="44"/>
@@ -48986,6 +49015,24 @@
     <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A49:B62"/>
+    <mergeCell ref="A15:M16"/>
+    <mergeCell ref="A31:M32"/>
+    <mergeCell ref="A33:B46"/>
+    <mergeCell ref="H33:I46"/>
+    <mergeCell ref="A47:M48"/>
+    <mergeCell ref="A63:M65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="N67:O67"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="N68:O68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="N69:O69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="N70:O70"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="N71:O71"/>
     <mergeCell ref="C77:D77"/>
     <mergeCell ref="C72:D72"/>
     <mergeCell ref="N72:O72"/>
@@ -48993,24 +49040,6 @@
     <mergeCell ref="C74:D74"/>
     <mergeCell ref="C75:D75"/>
     <mergeCell ref="C76:D76"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="N69:O69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="N70:O70"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="N71:O71"/>
-    <mergeCell ref="A63:M65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="N67:O67"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="N68:O68"/>
-    <mergeCell ref="A49:B62"/>
-    <mergeCell ref="A15:M16"/>
-    <mergeCell ref="A31:M32"/>
-    <mergeCell ref="A33:B46"/>
-    <mergeCell ref="H33:I46"/>
-    <mergeCell ref="A47:M48"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.39409448818897641" bottom="0.39409448818897641" header="0" footer="0"/>
   <headerFooter>
@@ -58112,8 +58141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMJ103"/>
   <sheetViews>
-    <sheetView topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="D96" sqref="D96"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -58132,7 +58161,8 @@
     <col min="12" max="12" width="10.75" style="4" customWidth="1"/>
     <col min="13" max="13" width="10.75" style="1" customWidth="1"/>
     <col min="14" max="14" width="10.75" style="48" customWidth="1"/>
-    <col min="15" max="16" width="10.75" style="4" customWidth="1"/>
+    <col min="15" max="15" width="10.75" style="4" customWidth="1"/>
+    <col min="16" max="16" width="10.75" style="44" customWidth="1"/>
     <col min="17" max="17" width="21.875" style="4" customWidth="1"/>
     <col min="18" max="18" width="10.75" style="4" customWidth="1"/>
     <col min="19" max="19" width="10.75" style="48" customWidth="1"/>
@@ -58193,6 +58223,7 @@
       <c r="O1" s="17" t="s">
         <v>66</v>
       </c>
+      <c r="P1" s="68"/>
       <c r="R1" s="29" t="s">
         <v>65</v>
       </c>
@@ -58237,7 +58268,7 @@
       <c r="BJ1" s="44"/>
       <c r="BK1" s="44"/>
     </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:63" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>29</v>
       </c>
@@ -58275,7 +58306,10 @@
       <c r="O2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="P2" s="1"/>
+      <c r="P2" s="48">
+        <f>Utente!D49</f>
+        <v>0</v>
+      </c>
       <c r="Q2" s="4" t="s">
         <v>30</v>
       </c>
@@ -58333,9 +58367,9 @@
       <c r="AK2" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="AL2" s="1">
-        <f>IF(AG2&lt;=0,0,AM2)</f>
-        <v>0</v>
+      <c r="AL2" s="67">
+        <f>IF(AM2&lt;=0,0,AM2)</f>
+        <v>8</v>
       </c>
       <c r="AM2" s="41">
         <v>8</v>
@@ -58396,7 +58430,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:63" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>36</v>
       </c>
@@ -58438,7 +58472,10 @@
       <c r="O3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="P3" s="1"/>
+      <c r="P3" s="48">
+        <f>Utente!D50</f>
+        <v>0</v>
+      </c>
       <c r="Q3" s="4" t="s">
         <v>37</v>
       </c>
@@ -58503,9 +58540,9 @@
       <c r="AK3" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="AL3" s="1">
-        <f>IF(AG2&lt;=0,0,AM3)</f>
-        <v>0</v>
+      <c r="AL3" s="67">
+        <f t="shared" ref="AL3:AL4" si="0">IF(AM3&lt;=0,0,AM3)</f>
+        <v>2</v>
       </c>
       <c r="AM3" s="41">
         <v>2</v>
@@ -58563,7 +58600,7 @@
         <v>-22.5</v>
       </c>
     </row>
-    <row r="4" spans="1:63" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:63" ht="15" x14ac:dyDescent="0.25">
       <c r="C4" s="4" t="s">
         <v>71</v>
       </c>
@@ -58595,7 +58632,7 @@
       <c r="K4" s="48">
         <v>4</v>
       </c>
-      <c r="P4" s="1"/>
+      <c r="P4" s="48"/>
       <c r="Q4" s="4" t="s">
         <v>71</v>
       </c>
@@ -58654,9 +58691,9 @@
       <c r="AK4" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="AL4" s="1">
-        <f>IF(AG2&lt;=0,0,AM4)</f>
-        <v>0</v>
+      <c r="AL4" s="67">
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="AM4" s="41">
         <v>2</v>
@@ -58689,7 +58726,7 @@
       </c>
       <c r="BB4" s="33"/>
     </row>
-    <row r="5" spans="1:63" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:63" ht="15" x14ac:dyDescent="0.25">
       <c r="C5" s="4" t="s">
         <v>74</v>
       </c>
@@ -58718,11 +58755,11 @@
       <c r="M5" s="1">
         <v>-3</v>
       </c>
-      <c r="N5" s="53">
-        <f>E5/6</f>
-        <v>18.333333333333332</v>
-      </c>
-      <c r="P5" s="1"/>
+      <c r="N5" s="70">
+        <f>_xlfn.FLOOR.MATH(E5/6)</f>
+        <v>18</v>
+      </c>
+      <c r="P5" s="48"/>
       <c r="Q5" s="4" t="s">
         <v>75</v>
       </c>
@@ -58784,9 +58821,9 @@
       <c r="AI5" s="1">
         <v>-3</v>
       </c>
-      <c r="AJ5" s="43">
-        <f>AG5/6</f>
-        <v>-3.3333333333333335</v>
+      <c r="AJ5" s="70">
+        <f>_xlfn.FLOOR.MATH(AG5/6)</f>
+        <v>-4</v>
       </c>
       <c r="AK5" s="33" t="s">
         <v>44</v>
@@ -58862,7 +58899,7 @@
       </c>
       <c r="I6" s="35"/>
       <c r="J6" s="24"/>
-      <c r="P6" s="1"/>
+      <c r="P6" s="48"/>
       <c r="Q6" s="15" t="s">
         <v>81</v>
       </c>
@@ -58956,17 +58993,17 @@
       </c>
       <c r="BB6" s="35"/>
     </row>
-    <row r="7" spans="1:63" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:63" ht="15" x14ac:dyDescent="0.25">
       <c r="C7" s="4" t="s">
         <v>70</v>
       </c>
       <c r="D7" s="1">
-        <f>IF(B2&lt;=0,0,(B2-40)*M5)</f>
-        <v>-240</v>
+        <f>IF(B2&lt;=0,0,(B2-40)*N5)</f>
+        <v>1440</v>
       </c>
       <c r="E7" s="48">
-        <f>(B2-40)*M5</f>
-        <v>-240</v>
+        <f>(B2-40)*N5</f>
+        <v>1440</v>
       </c>
       <c r="F7" s="33" t="s">
         <v>44</v>
@@ -58980,7 +59017,7 @@
         <v>1096</v>
       </c>
       <c r="I7" s="33"/>
-      <c r="P7" s="1"/>
+      <c r="P7" s="48"/>
       <c r="Q7" s="4" t="s">
         <v>7</v>
       </c>
@@ -59009,13 +59046,13 @@
       <c r="AE7" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="AF7" s="1">
-        <f>IF(AD2&lt;=0,0,(AD2-25)*AI5)</f>
-        <v>0</v>
-      </c>
-      <c r="AG7" s="41">
-        <f>(AD2-25)*AI5</f>
-        <v>75</v>
+      <c r="AF7" s="67">
+        <f>IF(AD2&lt;=0,0,(AD2-25)*AJ5)</f>
+        <v>0</v>
+      </c>
+      <c r="AG7" s="67">
+        <f>(AD2-25)*AJ5</f>
+        <v>100</v>
       </c>
       <c r="AJ7" s="41"/>
       <c r="AK7" s="33" t="s">
@@ -59079,7 +59116,7 @@
         <v>102</v>
       </c>
       <c r="I8" s="33"/>
-      <c r="P8" s="1"/>
+      <c r="P8" s="48"/>
       <c r="Q8" s="15" t="s">
         <v>34</v>
       </c>
@@ -59153,7 +59190,7 @@
       </c>
       <c r="BB8" s="33"/>
     </row>
-    <row r="9" spans="1:63" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:63" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C9" s="4" t="s">
         <v>7</v>
       </c>
@@ -59168,15 +59205,15 @@
       <c r="F9" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="1">
-        <f>IF(B5&lt;=0,0,H9)</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="48">
-        <v>1</v>
+      <c r="G9" s="67">
+        <f>IF(B2&lt;=0,0,H9)</f>
+        <v>2</v>
+      </c>
+      <c r="H9" s="67">
+        <v>2</v>
       </c>
       <c r="I9" s="33"/>
-      <c r="P9" s="1"/>
+      <c r="P9" s="48"/>
       <c r="Q9" s="15"/>
       <c r="R9" s="1"/>
       <c r="W9" s="33" t="s">
@@ -59197,8 +59234,8 @@
       <c r="AK9" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="AL9" s="1">
-        <f>IF(AD2&lt;=0,0,AM2)</f>
+      <c r="AL9" s="69">
+        <f>IF(AD2&lt;=0,0,AM9)</f>
         <v>0</v>
       </c>
       <c r="AM9" s="41">
@@ -59225,12 +59262,11 @@
     </row>
     <row r="10" spans="1:63" x14ac:dyDescent="0.2">
       <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
       <c r="Q10" s="15"/>
       <c r="R10" s="15"/>
       <c r="T10" s="15"/>
     </row>
-    <row r="11" spans="1:63" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:63" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>29</v>
       </c>
@@ -59268,7 +59304,10 @@
       <c r="O11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="P11" s="1"/>
+      <c r="P11" s="48">
+        <f>Utente!D52</f>
+        <v>0</v>
+      </c>
       <c r="Q11" s="4" t="s">
         <v>30</v>
       </c>
@@ -59326,9 +59365,9 @@
       <c r="AK11" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="AL11" s="1">
-        <f>IF(AG11&lt;=0,0,AM11)</f>
-        <v>0</v>
+      <c r="AL11" s="67">
+        <f>IF(AM11&lt;=0,0,AM11)</f>
+        <v>8</v>
       </c>
       <c r="AM11" s="41">
         <v>8</v>
@@ -59389,7 +59428,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:63" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:63" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>36</v>
       </c>
@@ -59431,7 +59470,10 @@
       <c r="O12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="P12" s="1"/>
+      <c r="P12" s="48">
+        <f>Utente!D53</f>
+        <v>0</v>
+      </c>
       <c r="Q12" s="4" t="s">
         <v>37</v>
       </c>
@@ -59496,9 +59538,9 @@
       <c r="AK12" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="AL12" s="1">
-        <f>IF(AG11&lt;=0,0,AM12)</f>
-        <v>0</v>
+      <c r="AL12" s="67">
+        <f t="shared" ref="AL12:AL13" si="1">IF(AM12&lt;=0,0,AM12)</f>
+        <v>2</v>
       </c>
       <c r="AM12" s="41">
         <v>2</v>
@@ -59556,7 +59598,7 @@
         <v>-22.5</v>
       </c>
     </row>
-    <row r="13" spans="1:63" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:63" ht="15" x14ac:dyDescent="0.25">
       <c r="C13" s="4" t="s">
         <v>71</v>
       </c>
@@ -59588,7 +59630,7 @@
       <c r="K13" s="48">
         <v>4</v>
       </c>
-      <c r="P13" s="1"/>
+      <c r="P13" s="48"/>
       <c r="Q13" s="4" t="s">
         <v>71</v>
       </c>
@@ -59647,9 +59689,9 @@
       <c r="AK13" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="AL13" s="1">
-        <f>IF(AG11&lt;=0,0,AM13)</f>
-        <v>0</v>
+      <c r="AL13" s="67">
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="AM13" s="41">
         <v>2</v>
@@ -59715,7 +59757,7 @@
         <f>E14/6</f>
         <v>-3.3333333333333335</v>
       </c>
-      <c r="P14" s="1"/>
+      <c r="P14" s="48"/>
       <c r="Q14" s="4" t="s">
         <v>75</v>
       </c>
@@ -59855,7 +59897,7 @@
       </c>
       <c r="I15" s="35"/>
       <c r="J15" s="24"/>
-      <c r="P15" s="1"/>
+      <c r="P15" s="48"/>
       <c r="Q15" s="15" t="s">
         <v>81</v>
       </c>
@@ -59973,7 +60015,7 @@
         <v>0</v>
       </c>
       <c r="I16" s="33"/>
-      <c r="P16" s="1"/>
+      <c r="P16" s="48"/>
       <c r="Q16" s="4" t="s">
         <v>7</v>
       </c>
@@ -60003,12 +60045,12 @@
         <v>70</v>
       </c>
       <c r="AF16" s="1">
-        <f>IF(AD11&lt;=0,0,(AD11-25)*AI14)</f>
+        <f>IF(AD11&lt;=0,0,(AD11-25)*AJ14)</f>
         <v>0</v>
       </c>
       <c r="AG16" s="41">
-        <f>(AD11-25)*AI14</f>
-        <v>75</v>
+        <f>(AD11-25)*AJ14</f>
+        <v>83.333333333333343</v>
       </c>
       <c r="AJ16" s="41"/>
       <c r="AK16" s="33" t="s">
@@ -60072,7 +60114,7 @@
         <v>-28</v>
       </c>
       <c r="I17" s="33"/>
-      <c r="P17" s="1"/>
+      <c r="P17" s="48"/>
       <c r="Q17" s="15" t="s">
         <v>34</v>
       </c>
@@ -60146,7 +60188,7 @@
       </c>
       <c r="BB17" s="33"/>
     </row>
-    <row r="18" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:56" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C18" s="4" t="s">
         <v>7</v>
       </c>
@@ -60169,7 +60211,7 @@
         <v>1</v>
       </c>
       <c r="I18" s="33"/>
-      <c r="P18" s="1"/>
+      <c r="P18" s="48"/>
       <c r="Q18" s="15"/>
       <c r="R18" s="1"/>
       <c r="W18" s="33" t="s">
@@ -60186,8 +60228,8 @@
       <c r="AK18" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="AL18" s="1">
-        <f>IF(AD11&lt;=0,0,AM11)</f>
+      <c r="AL18" s="69">
+        <f>IF(AD11&lt;=0,0,AM18)</f>
         <v>0</v>
       </c>
       <c r="AM18" s="41">
@@ -60216,7 +60258,10 @@
       <c r="O19" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="P19" s="1"/>
+      <c r="P19" s="48">
+        <f>Utente!D55</f>
+        <v>0</v>
+      </c>
       <c r="Q19" s="4" t="s">
         <v>30</v>
       </c>
@@ -60361,7 +60406,10 @@
       <c r="O20" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="P20" s="1"/>
+      <c r="P20" s="48">
+        <f>Utente!D56</f>
+        <v>0</v>
+      </c>
       <c r="Q20" s="4" t="s">
         <v>37</v>
       </c>
@@ -60532,7 +60580,7 @@
       <c r="K21" s="48">
         <v>2</v>
       </c>
-      <c r="P21" s="1"/>
+      <c r="P21" s="48"/>
       <c r="Q21" s="4" t="s">
         <v>71</v>
       </c>
@@ -60658,7 +60706,7 @@
       <c r="K22" s="48">
         <v>4</v>
       </c>
-      <c r="P22" s="1"/>
+      <c r="P22" s="48"/>
       <c r="Q22" s="4" t="s">
         <v>75</v>
       </c>
@@ -60806,7 +60854,7 @@
         <f>E23/6</f>
         <v>-3.3333333333333335</v>
       </c>
-      <c r="P23" s="1"/>
+      <c r="P23" s="48"/>
       <c r="Q23" s="15" t="s">
         <v>81</v>
       </c>
@@ -60924,7 +60972,7 @@
       </c>
       <c r="I24" s="35"/>
       <c r="J24" s="24"/>
-      <c r="P24" s="1"/>
+      <c r="P24" s="48"/>
       <c r="Q24" s="4" t="s">
         <v>7</v>
       </c>
@@ -61024,7 +61072,7 @@
         <v>0</v>
       </c>
       <c r="I25" s="33"/>
-      <c r="P25" s="1"/>
+      <c r="P25" s="48"/>
       <c r="Q25" s="15" t="s">
         <v>34</v>
       </c>
@@ -61122,7 +61170,7 @@
         <v>-28</v>
       </c>
       <c r="I26" s="33"/>
-      <c r="P26" s="1"/>
+      <c r="P26" s="48"/>
       <c r="Q26" s="15"/>
       <c r="R26" s="1"/>
       <c r="W26" s="33" t="s">
@@ -61227,7 +61275,10 @@
       <c r="O28" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="P28" s="1"/>
+      <c r="P28" s="48">
+        <f>Utente!D58</f>
+        <v>0</v>
+      </c>
       <c r="Q28" s="4" t="s">
         <v>30</v>
       </c>
@@ -61372,7 +61423,10 @@
       <c r="O29" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="P29" s="1"/>
+      <c r="P29" s="48">
+        <f>Utente!D59</f>
+        <v>0</v>
+      </c>
       <c r="Q29" s="4" t="s">
         <v>37</v>
       </c>
@@ -61543,7 +61597,7 @@
       <c r="K30" s="48">
         <v>2</v>
       </c>
-      <c r="P30" s="1"/>
+      <c r="P30" s="48"/>
       <c r="Q30" s="4" t="s">
         <v>71</v>
       </c>
@@ -61669,7 +61723,7 @@
       <c r="K31" s="48">
         <v>4</v>
       </c>
-      <c r="P31" s="1"/>
+      <c r="P31" s="48"/>
       <c r="Q31" s="4" t="s">
         <v>75</v>
       </c>
@@ -61817,7 +61871,7 @@
         <f>E32/6</f>
         <v>-3.3333333333333335</v>
       </c>
-      <c r="P32" s="1"/>
+      <c r="P32" s="48"/>
       <c r="Q32" s="15" t="s">
         <v>81</v>
       </c>
@@ -61935,7 +61989,7 @@
       </c>
       <c r="I33" s="35"/>
       <c r="J33" s="24"/>
-      <c r="P33" s="1"/>
+      <c r="P33" s="48"/>
       <c r="Q33" s="4" t="s">
         <v>7</v>
       </c>
@@ -62035,7 +62089,7 @@
         <v>0</v>
       </c>
       <c r="I34" s="33"/>
-      <c r="P34" s="1"/>
+      <c r="P34" s="48"/>
       <c r="Q34" s="15" t="s">
         <v>34</v>
       </c>
@@ -62133,7 +62187,7 @@
         <v>-28</v>
       </c>
       <c r="I35" s="33"/>
-      <c r="P35" s="1"/>
+      <c r="P35" s="48"/>
       <c r="Q35" s="15"/>
       <c r="R35" s="1"/>
       <c r="W35" s="33" t="s">
@@ -62272,7 +62326,10 @@
       <c r="O38" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="P38" s="1"/>
+      <c r="P38" s="48">
+        <f>Utente!D61</f>
+        <v>0</v>
+      </c>
       <c r="Q38" s="4" t="s">
         <v>30</v>
       </c>
@@ -62435,7 +62492,10 @@
       <c r="O39" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="P39" s="1"/>
+      <c r="P39" s="48">
+        <f>Utente!D62</f>
+        <v>0</v>
+      </c>
       <c r="Q39" s="4" t="s">
         <v>37</v>
       </c>
@@ -62592,7 +62652,7 @@
       <c r="K40" s="48">
         <v>4</v>
       </c>
-      <c r="P40" s="1"/>
+      <c r="P40" s="48"/>
       <c r="Q40" s="4" t="s">
         <v>71</v>
       </c>
@@ -62719,7 +62779,7 @@
         <f>E41/6</f>
         <v>-3.3333333333333335</v>
       </c>
-      <c r="P41" s="1"/>
+      <c r="P41" s="48"/>
       <c r="Q41" s="4" t="s">
         <v>75</v>
       </c>
@@ -62859,7 +62919,7 @@
       </c>
       <c r="I42" s="35"/>
       <c r="J42" s="24"/>
-      <c r="P42" s="1"/>
+      <c r="P42" s="48"/>
       <c r="Q42" s="15" t="s">
         <v>81</v>
       </c>
@@ -62977,7 +63037,7 @@
         <v>0</v>
       </c>
       <c r="I43" s="33"/>
-      <c r="P43" s="1"/>
+      <c r="P43" s="48"/>
       <c r="Q43" s="4" t="s">
         <v>7</v>
       </c>
@@ -63076,7 +63136,7 @@
         <v>-28</v>
       </c>
       <c r="I44" s="33"/>
-      <c r="P44" s="1"/>
+      <c r="P44" s="48"/>
       <c r="Q44" s="15" t="s">
         <v>34</v>
       </c>
@@ -63173,7 +63233,7 @@
         <v>1</v>
       </c>
       <c r="I45" s="33"/>
-      <c r="P45" s="1"/>
+      <c r="P45" s="48"/>
       <c r="Q45" s="15"/>
       <c r="R45" s="1"/>
       <c r="W45" s="33" t="s">
@@ -63254,7 +63314,10 @@
       <c r="O47" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="P47" s="1"/>
+      <c r="P47" s="48">
+        <f>Utente!F49</f>
+        <v>0</v>
+      </c>
       <c r="Q47" s="4" t="s">
         <v>30</v>
       </c>
@@ -63417,7 +63480,10 @@
       <c r="O48" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="P48" s="1"/>
+      <c r="P48" s="48">
+        <f>Utente!F50</f>
+        <v>0</v>
+      </c>
       <c r="Q48" s="4" t="s">
         <v>37</v>
       </c>
@@ -63574,7 +63640,7 @@
       <c r="K49" s="48">
         <v>4</v>
       </c>
-      <c r="P49" s="1"/>
+      <c r="P49" s="48"/>
       <c r="Q49" s="4" t="s">
         <v>71</v>
       </c>
@@ -63701,7 +63767,7 @@
         <f>E50/6</f>
         <v>-3.3333333333333335</v>
       </c>
-      <c r="P50" s="1"/>
+      <c r="P50" s="48"/>
       <c r="Q50" s="4" t="s">
         <v>75</v>
       </c>
@@ -63841,7 +63907,7 @@
       </c>
       <c r="I51" s="35"/>
       <c r="J51" s="24"/>
-      <c r="P51" s="1"/>
+      <c r="P51" s="48"/>
       <c r="Q51" s="15" t="s">
         <v>81</v>
       </c>
@@ -63959,7 +64025,7 @@
         <v>0</v>
       </c>
       <c r="I52" s="33"/>
-      <c r="P52" s="1"/>
+      <c r="P52" s="48"/>
       <c r="Q52" s="4" t="s">
         <v>7</v>
       </c>
@@ -64058,7 +64124,7 @@
         <v>-28</v>
       </c>
       <c r="I53" s="33"/>
-      <c r="P53" s="1"/>
+      <c r="P53" s="48"/>
       <c r="Q53" s="15" t="s">
         <v>34</v>
       </c>
@@ -64155,7 +64221,7 @@
         <v>1</v>
       </c>
       <c r="I54" s="33"/>
-      <c r="P54" s="1"/>
+      <c r="P54" s="48"/>
       <c r="Q54" s="15"/>
       <c r="R54" s="1"/>
       <c r="W54" s="33" t="s">
@@ -64236,7 +64302,10 @@
       <c r="O56" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="P56" s="1"/>
+      <c r="P56" s="48">
+        <f>Utente!F52</f>
+        <v>0</v>
+      </c>
       <c r="Q56" s="4" t="s">
         <v>30</v>
       </c>
@@ -64399,7 +64468,10 @@
       <c r="O57" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="P57" s="1"/>
+      <c r="P57" s="48">
+        <f>Utente!F53</f>
+        <v>0</v>
+      </c>
       <c r="Q57" s="4" t="s">
         <v>37</v>
       </c>
@@ -64556,7 +64628,7 @@
       <c r="K58" s="48">
         <v>4</v>
       </c>
-      <c r="P58" s="1"/>
+      <c r="P58" s="48"/>
       <c r="Q58" s="4" t="s">
         <v>71</v>
       </c>
@@ -64683,7 +64755,7 @@
         <f>E59/6</f>
         <v>-3.3333333333333335</v>
       </c>
-      <c r="P59" s="1"/>
+      <c r="P59" s="48"/>
       <c r="Q59" s="4" t="s">
         <v>75</v>
       </c>
@@ -64823,7 +64895,7 @@
       </c>
       <c r="I60" s="35"/>
       <c r="J60" s="24"/>
-      <c r="P60" s="1"/>
+      <c r="P60" s="48"/>
       <c r="Q60" s="15" t="s">
         <v>81</v>
       </c>
@@ -64941,7 +65013,7 @@
         <v>0</v>
       </c>
       <c r="I61" s="33"/>
-      <c r="P61" s="1"/>
+      <c r="P61" s="48"/>
       <c r="Q61" s="4" t="s">
         <v>7</v>
       </c>
@@ -65040,7 +65112,7 @@
         <v>-28</v>
       </c>
       <c r="I62" s="33"/>
-      <c r="P62" s="1"/>
+      <c r="P62" s="48"/>
       <c r="Q62" s="15" t="s">
         <v>34</v>
       </c>
@@ -65137,7 +65209,7 @@
         <v>1</v>
       </c>
       <c r="I63" s="33"/>
-      <c r="P63" s="1"/>
+      <c r="P63" s="48"/>
       <c r="Q63" s="15"/>
       <c r="R63" s="1"/>
       <c r="W63" s="33" t="s">
@@ -65218,7 +65290,10 @@
       <c r="O65" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="P65" s="1"/>
+      <c r="P65" s="48">
+        <f>Utente!F55</f>
+        <v>0</v>
+      </c>
       <c r="Q65" s="4" t="s">
         <v>30</v>
       </c>
@@ -65381,7 +65456,10 @@
       <c r="O66" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="P66" s="1"/>
+      <c r="P66" s="48">
+        <f>Utente!F56</f>
+        <v>0</v>
+      </c>
       <c r="Q66" s="4" t="s">
         <v>37</v>
       </c>
@@ -65538,7 +65616,7 @@
       <c r="K67" s="48">
         <v>4</v>
       </c>
-      <c r="P67" s="1"/>
+      <c r="P67" s="48"/>
       <c r="Q67" s="4" t="s">
         <v>71</v>
       </c>
@@ -65665,7 +65743,7 @@
         <f>E68/6</f>
         <v>-3.3333333333333335</v>
       </c>
-      <c r="P68" s="1"/>
+      <c r="P68" s="48"/>
       <c r="Q68" s="4" t="s">
         <v>75</v>
       </c>
@@ -65805,7 +65883,7 @@
       </c>
       <c r="I69" s="35"/>
       <c r="J69" s="24"/>
-      <c r="P69" s="1"/>
+      <c r="P69" s="48"/>
       <c r="Q69" s="15" t="s">
         <v>81</v>
       </c>
@@ -65923,7 +66001,7 @@
         <v>0</v>
       </c>
       <c r="I70" s="33"/>
-      <c r="P70" s="1"/>
+      <c r="P70" s="48"/>
       <c r="Q70" s="4" t="s">
         <v>7</v>
       </c>
@@ -66022,7 +66100,7 @@
         <v>-28</v>
       </c>
       <c r="I71" s="33"/>
-      <c r="P71" s="1"/>
+      <c r="P71" s="48"/>
       <c r="Q71" s="15" t="s">
         <v>34</v>
       </c>
@@ -66119,7 +66197,7 @@
         <v>1</v>
       </c>
       <c r="I72" s="33"/>
-      <c r="P72" s="1"/>
+      <c r="P72" s="48"/>
       <c r="Q72" s="15"/>
       <c r="R72" s="1"/>
       <c r="W72" s="33" t="s">
@@ -66200,7 +66278,10 @@
       <c r="O74" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="P74" s="1"/>
+      <c r="P74" s="48">
+        <f>Utente!F58</f>
+        <v>0</v>
+      </c>
       <c r="Q74" s="4" t="s">
         <v>30</v>
       </c>
@@ -66363,7 +66444,10 @@
       <c r="O75" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="P75" s="1"/>
+      <c r="P75" s="48">
+        <f>Utente!F59</f>
+        <v>0</v>
+      </c>
       <c r="Q75" s="4" t="s">
         <v>37</v>
       </c>
@@ -66520,7 +66604,7 @@
       <c r="K76" s="48">
         <v>4</v>
       </c>
-      <c r="P76" s="1"/>
+      <c r="P76" s="48"/>
       <c r="Q76" s="4" t="s">
         <v>71</v>
       </c>
@@ -66647,7 +66731,7 @@
         <f>E77/6</f>
         <v>-3.3333333333333335</v>
       </c>
-      <c r="P77" s="1"/>
+      <c r="P77" s="48"/>
       <c r="Q77" s="4" t="s">
         <v>75</v>
       </c>
@@ -66787,7 +66871,7 @@
       </c>
       <c r="I78" s="35"/>
       <c r="J78" s="24"/>
-      <c r="P78" s="1"/>
+      <c r="P78" s="48"/>
       <c r="Q78" s="15" t="s">
         <v>81</v>
       </c>
@@ -66905,7 +66989,7 @@
         <v>0</v>
       </c>
       <c r="I79" s="33"/>
-      <c r="P79" s="1"/>
+      <c r="P79" s="48"/>
       <c r="Q79" s="4" t="s">
         <v>7</v>
       </c>
@@ -67004,7 +67088,7 @@
         <v>-28</v>
       </c>
       <c r="I80" s="33"/>
-      <c r="P80" s="1"/>
+      <c r="P80" s="48"/>
       <c r="Q80" s="15" t="s">
         <v>34</v>
       </c>
@@ -67101,7 +67185,7 @@
         <v>1</v>
       </c>
       <c r="I81" s="33"/>
-      <c r="P81" s="1"/>
+      <c r="P81" s="48"/>
       <c r="Q81" s="15"/>
       <c r="R81" s="1"/>
       <c r="W81" s="33" t="s">
@@ -67182,7 +67266,10 @@
       <c r="O83" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="P83" s="1"/>
+      <c r="P83" s="48">
+        <f>Utente!F61</f>
+        <v>0</v>
+      </c>
       <c r="Q83" s="4" t="s">
         <v>30</v>
       </c>
@@ -67345,7 +67432,10 @@
       <c r="O84" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="P84" s="1"/>
+      <c r="P84" s="48">
+        <f>Utente!F62</f>
+        <v>0</v>
+      </c>
       <c r="Q84" s="4" t="s">
         <v>37</v>
       </c>
@@ -67502,7 +67592,7 @@
       <c r="K85" s="48">
         <v>4</v>
       </c>
-      <c r="P85" s="1"/>
+      <c r="P85" s="48"/>
       <c r="Q85" s="4" t="s">
         <v>71</v>
       </c>
@@ -67629,7 +67719,7 @@
         <f>E86/6</f>
         <v>-3.3333333333333335</v>
       </c>
-      <c r="P86" s="1"/>
+      <c r="P86" s="48"/>
       <c r="Q86" s="4" t="s">
         <v>75</v>
       </c>
@@ -67769,7 +67859,7 @@
       </c>
       <c r="I87" s="35"/>
       <c r="J87" s="24"/>
-      <c r="P87" s="1"/>
+      <c r="P87" s="48"/>
       <c r="Q87" s="15" t="s">
         <v>81</v>
       </c>
@@ -67887,7 +67977,7 @@
         <v>0</v>
       </c>
       <c r="I88" s="33"/>
-      <c r="P88" s="1"/>
+      <c r="P88" s="48"/>
       <c r="Q88" s="4" t="s">
         <v>7</v>
       </c>
@@ -67986,7 +68076,7 @@
         <v>-28</v>
       </c>
       <c r="I89" s="33"/>
-      <c r="P89" s="1"/>
+      <c r="P89" s="48"/>
       <c r="Q89" s="15" t="s">
         <v>34</v>
       </c>
@@ -68083,7 +68173,7 @@
         <v>1</v>
       </c>
       <c r="I90" s="33"/>
-      <c r="P90" s="1"/>
+      <c r="P90" s="48"/>
       <c r="Q90" s="15"/>
       <c r="R90" s="1"/>
       <c r="W90" s="33" t="s">
@@ -68388,7 +68478,7 @@
       </c>
       <c r="D99" s="36">
         <f>(D7+D16+D25+D34+D43+D52+D61+D70+D79+D88)/650</f>
-        <v>-0.36923076923076925</v>
+        <v>2.2153846153846155</v>
       </c>
       <c r="O99" s="15"/>
       <c r="Q99" s="4" t="s">
@@ -68421,7 +68511,7 @@
       </c>
       <c r="BC99" s="38">
         <f>D99+R99+AF98+AT98</f>
-        <v>-0.36923076923076925</v>
+        <v>2.2153846153846155</v>
       </c>
     </row>
     <row r="100" spans="3:55" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fascione and zoccolo cells fixed
</commit_message>
<xml_diff>
--- a/ArnaldoDiBianco/Lista_materiale3.xlsx
+++ b/ArnaldoDiBianco/Lista_materiale3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sources\GitHub\DonBruno\ArnaldoDiBianco\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB7034E-4B4A-493D-8FD9-BEF9F9DA0B35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3731B48B-22F8-46F2-8B07-004DA8DEC4F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11175" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11175" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Utente" sheetId="1" r:id="rId1"/>
@@ -1670,8 +1670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMH1048576"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="E70" sqref="E70"/>
+    <sheetView topLeftCell="H34" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1989,9 +1989,7 @@
       <c r="J17" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="K17" s="3">
-        <v>120</v>
-      </c>
+      <c r="K17" s="3"/>
       <c r="L17" s="2" t="s">
         <v>0</v>
       </c>
@@ -2014,9 +2012,7 @@
       <c r="J18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K18" s="3">
-        <v>130</v>
-      </c>
+      <c r="K18" s="3"/>
       <c r="L18" s="2" t="s">
         <v>1</v>
       </c>
@@ -2272,7 +2268,9 @@
       <c r="J33" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="K33" s="3"/>
+      <c r="K33" s="3">
+        <v>120</v>
+      </c>
       <c r="L33" s="2" t="s">
         <v>0</v>
       </c>
@@ -2295,7 +2293,9 @@
       <c r="J34" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K34" s="3"/>
+      <c r="K34" s="3">
+        <v>130</v>
+      </c>
       <c r="L34" s="2" t="s">
         <v>1</v>
       </c>
@@ -4971,7 +4971,7 @@
       <c r="O68" s="63"/>
       <c r="P68" s="45">
         <f>Finestre!BA63</f>
-        <v>1.1046153846153846</v>
+        <v>0.72307692307692306</v>
       </c>
       <c r="Q68" s="44"/>
       <c r="R68" s="44"/>
@@ -5989,7 +5989,7 @@
       <c r="D69" s="62"/>
       <c r="E69" s="50">
         <f>P67+P68</f>
-        <v>1.1046153846153846</v>
+        <v>0.72307692307692306</v>
       </c>
       <c r="I69" s="44"/>
       <c r="N69" s="66" t="s">
@@ -7016,7 +7016,7 @@
       <c r="D70" s="62"/>
       <c r="E70" s="50">
         <f>P71+P72</f>
-        <v>0.18153846153846154</v>
+        <v>0</v>
       </c>
       <c r="I70" s="44"/>
       <c r="N70" s="63" t="s">
@@ -7025,7 +7025,7 @@
       <c r="O70" s="63"/>
       <c r="P70" s="45">
         <f>Finestre!BA65</f>
-        <v>0</v>
+        <v>0.15230769230769231</v>
       </c>
       <c r="Q70" s="44"/>
       <c r="R70" s="44"/>
@@ -9070,7 +9070,7 @@
       <c r="D72" s="62"/>
       <c r="E72" s="50">
         <f>P69+P70</f>
-        <v>0</v>
+        <v>0.15230769230769231</v>
       </c>
       <c r="I72" s="44"/>
       <c r="J72" s="44"/>
@@ -9080,7 +9080,7 @@
       <c r="O72" s="63"/>
       <c r="P72" s="45">
         <f>Finestre!BA67</f>
-        <v>0.18153846153846154</v>
+        <v>0</v>
       </c>
       <c r="Q72" s="44"/>
       <c r="R72" s="44"/>
@@ -10098,7 +10098,7 @@
       <c r="D73" s="64"/>
       <c r="E73" s="49">
         <f>Finestre!BA66</f>
-        <v>0</v>
+        <v>0.15230769230769231</v>
       </c>
       <c r="I73" s="44"/>
       <c r="J73" s="44"/>
@@ -50371,9 +50371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMJ69"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="W1" sqref="W1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -50505,21 +50503,21 @@
       </c>
       <c r="B2" s="23">
         <f>Utente!K17</f>
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="23">
         <f>B2+(2*B3)</f>
-        <v>380</v>
+        <v>0</v>
       </c>
       <c r="F2" s="13" t="s">
         <v>31</v>
       </c>
       <c r="G2" s="14">
         <f>IF(B2&lt;=0,0,H2)</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="H2" s="57">
         <v>12</v>
@@ -50529,7 +50527,7 @@
       </c>
       <c r="J2" s="14">
         <f>IF(B2&lt;=0,0,K2)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K2" s="57">
         <v>2</v>
@@ -50617,32 +50615,32 @@
       </c>
       <c r="AL2" s="23">
         <f>Utente!K33</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="AM2" s="16" t="s">
         <v>30</v>
       </c>
       <c r="AN2" s="23">
         <f>AL2+(2*AL3)</f>
-        <v>0</v>
+        <v>380</v>
       </c>
       <c r="AP2" s="13" t="s">
         <v>34</v>
       </c>
       <c r="AQ2" s="14">
         <f>IF(AR2&lt;=0,0,AL2-21)</f>
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="AR2" s="57">
         <f>AL2-21</f>
-        <v>-21</v>
+        <v>99</v>
       </c>
       <c r="AS2" s="13" t="s">
         <v>31</v>
       </c>
       <c r="AT2" s="14">
         <f>IF(AL2&lt;=0,0,AU2)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AU2" s="57">
         <v>8</v>
@@ -50652,7 +50650,7 @@
       </c>
       <c r="AW2" s="14">
         <f>IF(AL2&lt;=0,0,AX2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX2" s="57">
         <v>1</v>
@@ -50688,25 +50686,25 @@
       </c>
       <c r="B3" s="23">
         <f>Utente!K18</f>
-        <v>130</v>
+        <v>0</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>37</v>
       </c>
       <c r="D3" s="23">
         <f>IF(E3&lt;=0,0,((B2-9)*2)+((B3-6)*4))</f>
-        <v>718</v>
+        <v>0</v>
       </c>
       <c r="E3" s="55">
         <f>((B2-9)*2)+((B3-6)*4)</f>
-        <v>718</v>
+        <v>-42</v>
       </c>
       <c r="F3" s="13" t="s">
         <v>38</v>
       </c>
       <c r="G3" s="14">
         <f>IF(B2&lt;=0,0,H3)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H3" s="57">
         <v>4</v>
@@ -50716,7 +50714,7 @@
       </c>
       <c r="J3" s="14">
         <f>IF(B2&lt;=0,0,K3)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K3" s="57">
         <v>1</v>
@@ -50812,36 +50810,36 @@
       </c>
       <c r="AL3" s="23">
         <f>Utente!K34</f>
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="AM3" s="16" t="s">
         <v>37</v>
       </c>
       <c r="AN3" s="24">
         <f>IF(AO3&lt;=0,0,((AL2-9)*2)+((AL3-6)*2))</f>
-        <v>0</v>
+        <v>470</v>
       </c>
       <c r="AO3" s="55">
         <f>((AL2-9)*2)+((AL3-6)*2)</f>
-        <v>-30</v>
+        <v>470</v>
       </c>
       <c r="AP3" s="13" t="s">
         <v>40</v>
       </c>
       <c r="AQ3" s="14">
         <f>IF(AR3&lt;=0,0,AL2-21)</f>
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="AR3" s="57">
         <f>AL2-21</f>
-        <v>-21</v>
+        <v>99</v>
       </c>
       <c r="AS3" s="13" t="s">
         <v>38</v>
       </c>
       <c r="AT3" s="14">
         <f>IF(AL2&lt;=0,0,AU3)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AU3" s="57">
         <v>3</v>
@@ -50851,7 +50849,7 @@
       </c>
       <c r="AW3" s="14">
         <f>IF(AL2&lt;=0,0,AX3)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AX3" s="57">
         <v>2</v>
@@ -50890,18 +50888,18 @@
       </c>
       <c r="D4" s="23">
         <f>IF(E4&lt;=0,0,B2-4)</f>
-        <v>116</v>
+        <v>0</v>
       </c>
       <c r="E4" s="55">
         <f>B2-4</f>
-        <v>116</v>
+        <v>-4</v>
       </c>
       <c r="F4" s="13" t="s">
         <v>43</v>
       </c>
       <c r="G4" s="14">
         <f>IF(B2&lt;=0,0,H4)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" s="57">
         <v>1</v>
@@ -50911,7 +50909,7 @@
       </c>
       <c r="J4" s="14">
         <f>IF(B2&lt;=0,0,K4)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K4" s="57">
         <v>2</v>
@@ -50994,18 +50992,18 @@
       </c>
       <c r="AN4" s="23">
         <f>IF(AO4&lt;=0,0,AL2-4)</f>
-        <v>0</v>
+        <v>116</v>
       </c>
       <c r="AO4" s="55">
         <f>AL2-4</f>
-        <v>-4</v>
+        <v>116</v>
       </c>
       <c r="AP4" s="16" t="s">
         <v>46</v>
       </c>
       <c r="AQ4" s="23">
         <f>IF(AL2&lt;=0,0,AR4)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AR4" s="57">
         <v>6</v>
@@ -51015,18 +51013,18 @@
       </c>
       <c r="AT4" s="14">
         <f>AN2+AN3</f>
-        <v>0</v>
+        <v>850</v>
       </c>
       <c r="AU4" s="57">
         <f>AN2+AN3</f>
-        <v>0</v>
+        <v>850</v>
       </c>
       <c r="AV4" s="13" t="s">
         <v>45</v>
       </c>
       <c r="AW4" s="14">
         <f>IF(AL2&lt;=0,0,AX4)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX4" s="57">
         <v>1</v>
@@ -51057,29 +51055,29 @@
       </c>
       <c r="D5" s="23">
         <f>IF(E5&lt;=0,0,B3-12)</f>
-        <v>118</v>
+        <v>0</v>
       </c>
       <c r="E5" s="55">
         <f>B3-12</f>
-        <v>118</v>
+        <v>-12</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>44</v>
       </c>
       <c r="G5" s="14">
         <f>D2+D3</f>
-        <v>1098</v>
+        <v>0</v>
       </c>
       <c r="H5" s="57">
         <f>D2+D3</f>
-        <v>1098</v>
+        <v>0</v>
       </c>
       <c r="I5" s="13" t="s">
         <v>49</v>
       </c>
       <c r="J5" s="14">
         <f>IF(B2&lt;=0,0,K5)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5" s="57">
         <v>1</v>
@@ -51142,11 +51140,11 @@
       </c>
       <c r="AT5" s="14">
         <f>IF(AU5&lt;=0,0,AL3-40)</f>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="AU5" s="57">
         <f>AL3-40</f>
-        <v>-40</v>
+        <v>90</v>
       </c>
       <c r="AV5" s="13"/>
       <c r="BA5" s="16" t="s">
@@ -51166,7 +51164,7 @@
       </c>
       <c r="D6" s="23">
         <f>IF(B2&lt;=0,0,E6)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E6" s="55">
         <v>4</v>
@@ -51176,18 +51174,18 @@
       </c>
       <c r="G6" s="14">
         <f>IF(H6&lt;=0,0,B3-40)</f>
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="H6" s="57">
         <f>B3-40</f>
-        <v>90</v>
+        <v>-40</v>
       </c>
       <c r="I6" s="13" t="s">
         <v>45</v>
       </c>
       <c r="J6" s="14">
         <f>IF(B2&lt;=0,0,K6)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6" s="57">
         <v>1</v>
@@ -51229,7 +51227,7 @@
       </c>
       <c r="AT6" s="14">
         <f>IF(AL2&lt;=0,0,AU6)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AU6" s="57">
         <v>2</v>
@@ -57910,7 +57908,7 @@
       </c>
       <c r="D63" s="27">
         <f>(D2+D8+D14+D20+D26+D32+D38+D44)/650</f>
-        <v>0.58461538461538465</v>
+        <v>0</v>
       </c>
       <c r="N63" s="16" t="s">
         <v>52</v>
@@ -57931,7 +57929,7 @@
       </c>
       <c r="AN63" s="27">
         <f>(AN2+AN8+AN14+AN20+AN26+AN32+AN38+AN44+AN50+AN56)/650</f>
-        <v>0</v>
+        <v>0.58461538461538465</v>
       </c>
       <c r="AV63"/>
       <c r="AW63"/>
@@ -57940,7 +57938,7 @@
       </c>
       <c r="BA63" s="27">
         <f>D64+O64+Z64+AN64</f>
-        <v>1.1046153846153846</v>
+        <v>0.72307692307692306</v>
       </c>
     </row>
     <row r="64" spans="1:58" x14ac:dyDescent="0.2">
@@ -57949,7 +57947,7 @@
       </c>
       <c r="D64" s="27">
         <f>(D3+D9+D15+D21+D27+D33+D39+D45)/650</f>
-        <v>1.1046153846153846</v>
+        <v>0</v>
       </c>
       <c r="N64" s="16" t="s">
         <v>54</v>
@@ -57970,7 +57968,7 @@
       </c>
       <c r="AN64" s="27">
         <f>(AN3+AN9+AN15+AN21+AN27+AN33+AN39+AN45+AN51+AN57)/650</f>
-        <v>0</v>
+        <v>0.72307692307692306</v>
       </c>
       <c r="AV64"/>
       <c r="AW64"/>
@@ -57988,7 +57986,7 @@
       </c>
       <c r="D65" s="27">
         <f>(D4+D10+D16+D22+D28+D34+D40+D46)/650</f>
-        <v>0.17846153846153845</v>
+        <v>0</v>
       </c>
       <c r="N65" s="16" t="s">
         <v>56</v>
@@ -58009,7 +58007,7 @@
       </c>
       <c r="AN65" s="27">
         <f>(AN4+AN10+AN16+AN22+AN28+AN34+AN40+AN46+AN52+AN58)/650</f>
-        <v>0</v>
+        <v>0.17846153846153845</v>
       </c>
       <c r="AV65"/>
       <c r="AW65"/>
@@ -58018,7 +58016,7 @@
       </c>
       <c r="BA65" s="27">
         <f>Z67+AN66</f>
-        <v>0</v>
+        <v>0.15230769230769231</v>
       </c>
     </row>
     <row r="66" spans="3:53" x14ac:dyDescent="0.2">
@@ -58027,7 +58025,7 @@
       </c>
       <c r="D66" s="27">
         <f>(D5+D11+D17+D23+D29+D35+D41+D47)/650</f>
-        <v>0.18153846153846154</v>
+        <v>0</v>
       </c>
       <c r="N66" s="16" t="s">
         <v>60</v>
@@ -58047,8 +58045,8 @@
         <v>58</v>
       </c>
       <c r="AN66" s="27">
-        <f>(AQ2+AQ7+AQ13+AQ19+AQ25+AQ31+AQ37+AQ43+AQ49+AQ55)/650</f>
-        <v>0</v>
+        <f>(AQ2+AQ8+AQ14+AQ20+AQ26+AQ32+AQ38+AQ44+AQ50+AQ56)/650</f>
+        <v>0.15230769230769231</v>
       </c>
       <c r="AV66"/>
       <c r="AW66"/>
@@ -58057,7 +58055,7 @@
       </c>
       <c r="BA66" s="27">
         <f>Z68+AN67</f>
-        <v>0</v>
+        <v>0.15230769230769231</v>
       </c>
     </row>
     <row r="67" spans="3:53" x14ac:dyDescent="0.2">
@@ -58066,7 +58064,7 @@
       </c>
       <c r="D67" s="28">
         <f>(G6+G12+G18+G24+G30+G36+G42+G48+G54+G60)/650</f>
-        <v>0.13846153846153847</v>
+        <v>0</v>
       </c>
       <c r="Y67" s="16" t="s">
         <v>58</v>
@@ -58079,8 +58077,8 @@
         <v>62</v>
       </c>
       <c r="AN67" s="27">
-        <f>(AQ2+AQ8+AQ14+AQ20+AQ26+AQ32+AQ38+AQ44+AQ50+AQ56)/650</f>
-        <v>0</v>
+        <f>(AQ3+AQ9+AQ15+AQ21+AQ27+AQ33+AQ39+AQ45+AQ51+AQ57)/650</f>
+        <v>0.15230769230769231</v>
       </c>
       <c r="AV67"/>
       <c r="AW67"/>
@@ -58089,7 +58087,7 @@
       </c>
       <c r="BA67" s="27">
         <f>Z66+D66</f>
-        <v>0.18153846153846154</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="3:53" x14ac:dyDescent="0.2">
@@ -58105,7 +58103,7 @@
       </c>
       <c r="AN68" s="27">
         <f>(AT5+AT11+AT17+AT23+AT29+AT35+AT41+AT47+AT53+AT59)/650</f>
-        <v>0</v>
+        <v>0.13846153846153847</v>
       </c>
       <c r="AZ68" s="26" t="s">
         <v>64</v>
@@ -58137,7 +58135,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMJ103"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="Z1" sqref="Z1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -68606,7 +68606,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AB60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>